<commit_message>
Stand Alone Script -> Added column for Findings in RTM
</commit_message>
<xml_diff>
--- a/Testing_Documents/RTM.xlsx
+++ b/Testing_Documents/RTM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004us9s\Desktop\Study\Projects\GitHubProjects\UI-Automation_Selenium\Doc_Functional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\z004us9s\Desktop\Study\Projects\GitHubProjects\UI-Automation_Selenium\Testing_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C68D99A5-9D87-425E-8FF2-6668DFC96D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DCF58E2-555C-4278-9152-08112C35EECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{03D95421-2E75-4A27-AEB0-F0766E2F4348}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Requirement ID</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>Validate multiple users login attempt</t>
+  </si>
+  <si>
+    <t>Findings/Bug</t>
+  </si>
+  <si>
+    <t>Working as Designed</t>
   </si>
 </sst>
 </file>
@@ -139,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -162,11 +168,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -174,6 +191,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0A3702A-1B3E-4BF3-9B1C-528A455BA5E6}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -520,9 +541,10 @@
     <col min="2" max="2" width="56" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="69.7265625" customWidth="1"/>
+    <col min="5" max="5" width="17.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -535,8 +557,11 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -549,8 +574,11 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -563,8 +591,11 @@
       <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -577,8 +608,11 @@
       <c r="D4" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="E4" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
@@ -591,8 +625,11 @@
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -604,6 +641,9 @@
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>